<commit_message>
Setup test order for Test11_CartPageMainOperation.py.
</commit_message>
<xml_diff>
--- a/Luma/tests/Test11_CartPageMainOperation.xlsx
+++ b/Luma/tests/Test11_CartPageMainOperation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-project\luma-repo\Luma\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CDCC60-3E42-4C0C-AD09-B725C82D7BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5D2895-46EF-4C27-92E7-F3B3C4E0AC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29085" yWindow="840" windowWidth="26970" windowHeight="6600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductPage_1" sheetId="2" r:id="rId1"/>
@@ -436,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36589AC9-DEC5-4883-9C60-48FF053B7C55}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E4937-24AA-49B1-9FA7-E9BCD1F12858}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>